<commit_message>
work on gamlss + weighing
</commit_message>
<xml_diff>
--- a/data/all_waves/weigh_data.xlsx
+++ b/data/all_waves/weigh_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anuschka/Documents/climatechange/climatechange/data/all_waves/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C4EA3B-3894-9148-9324-956F074CF4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9127283F-11D7-1440-9FC1-7025A53D1BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="15700" xr2:uid="{589232E4-3D71-D747-A62A-14D4E3B0C8AE}"/>
   </bookViews>
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9464F51-D6CA-254C-B404-8BB877CB06E8}">
   <dimension ref="A1:W19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T29" sqref="T29"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -555,39 +555,39 @@
         <v>7441337</v>
       </c>
       <c r="E2">
-        <f>C2/W2</f>
+        <f t="shared" ref="E2:E19" si="0">C2/W2</f>
         <v>0.49430082933354574</v>
       </c>
       <c r="F2" s="1">
-        <f>D2/W2</f>
+        <f t="shared" ref="F2:F19" si="1">D2/W2</f>
         <v>0.50569917066645431</v>
       </c>
       <c r="G2">
         <v>3974318</v>
       </c>
       <c r="H2">
-        <f>G2/W2</f>
+        <f t="shared" ref="H2:H19" si="2">G2/W2</f>
         <v>0.27008712501056747</v>
       </c>
       <c r="I2">
         <v>3362751</v>
       </c>
       <c r="J2">
-        <f>I2/W2</f>
+        <f t="shared" ref="J2:J19" si="3">I2/W2</f>
         <v>0.22852618983091208</v>
       </c>
       <c r="K2">
         <v>2282716</v>
       </c>
       <c r="L2">
-        <f>K2/W2</f>
+        <f t="shared" ref="L2:L19" si="4">K2/W2</f>
         <v>0.15512905652130066</v>
       </c>
       <c r="M2">
         <v>2367802</v>
       </c>
       <c r="N2">
-        <f>M2/W2</f>
+        <f t="shared" ref="N2:N19" si="5">M2/W2</f>
         <v>0.16091133995172799</v>
       </c>
       <c r="W2">
@@ -608,39 +608,39 @@
         <v>7648728</v>
       </c>
       <c r="E3">
-        <f>C3/W3</f>
+        <f t="shared" si="0"/>
         <v>0.49443769147638827</v>
       </c>
       <c r="F3" s="1">
-        <f>D3/W3</f>
+        <f t="shared" si="1"/>
         <v>0.50556230852361173</v>
       </c>
       <c r="G3">
         <v>3828528</v>
       </c>
       <c r="H3">
-        <f>G3/W3</f>
+        <f t="shared" si="2"/>
         <v>0.25305638452920354</v>
       </c>
       <c r="I3">
         <v>3605015</v>
       </c>
       <c r="J3">
-        <f>I3/W3</f>
+        <f t="shared" si="3"/>
         <v>0.23828271912169555</v>
       </c>
       <c r="K3">
         <v>2429065</v>
       </c>
       <c r="L3">
-        <f>K3/W3</f>
+        <f t="shared" si="4"/>
         <v>0.16055528565715854</v>
       </c>
       <c r="M3">
         <v>2491681</v>
       </c>
       <c r="N3">
-        <f>M3/W3</f>
+        <f t="shared" si="5"/>
         <v>0.16469405088851655</v>
       </c>
       <c r="W3">
@@ -661,39 +661,39 @@
         <v>7703914</v>
       </c>
       <c r="E4">
-        <f>C4/W4</f>
+        <f t="shared" si="0"/>
         <v>0.49446669775319962</v>
       </c>
       <c r="F4" s="1">
-        <f>D4/W4</f>
+        <f t="shared" si="1"/>
         <v>0.50553330224680038</v>
       </c>
       <c r="G4">
         <v>3771688</v>
       </c>
       <c r="H4">
-        <f>G4/W4</f>
+        <f t="shared" si="2"/>
         <v>0.2474993736540452</v>
       </c>
       <c r="I4">
         <v>3605434</v>
       </c>
       <c r="J4">
-        <f>I4/W4</f>
+        <f t="shared" si="3"/>
         <v>0.23658973296598204</v>
       </c>
       <c r="K4">
         <v>2537408</v>
       </c>
       <c r="L4">
-        <f>K4/W4</f>
+        <f t="shared" si="4"/>
         <v>0.16650552503408647</v>
       </c>
       <c r="M4">
         <v>2523208</v>
       </c>
       <c r="N4">
-        <f>M4/W4</f>
+        <f t="shared" si="5"/>
         <v>0.16557371648950711</v>
       </c>
       <c r="W4">
@@ -714,39 +714,39 @@
         <v>7796640</v>
       </c>
       <c r="E5">
-        <f>C5/W5</f>
+        <f t="shared" si="0"/>
         <v>0.49451644638184267</v>
       </c>
       <c r="F5" s="1">
-        <f>D5/W5</f>
+        <f t="shared" si="1"/>
         <v>0.50548355361815733</v>
       </c>
       <c r="G5">
         <v>3638804</v>
       </c>
       <c r="H5">
-        <f>G5/W5</f>
+        <f t="shared" si="2"/>
         <v>0.23591644308830026</v>
       </c>
       <c r="I5">
         <v>3640905</v>
       </c>
       <c r="J5">
-        <f>I5/W5</f>
+        <f t="shared" si="3"/>
         <v>0.23605265829717892</v>
       </c>
       <c r="K5">
         <v>2719560</v>
       </c>
       <c r="L5">
-        <f>K5/W5</f>
+        <f t="shared" si="4"/>
         <v>0.17631862611045218</v>
       </c>
       <c r="M5">
         <v>2575811</v>
       </c>
       <c r="N5">
-        <f>M5/W5</f>
+        <f t="shared" si="5"/>
         <v>0.16699887358256113</v>
       </c>
       <c r="U5">
@@ -773,39 +773,39 @@
         <v>8017633</v>
       </c>
       <c r="E6">
-        <f>C6/W6</f>
+        <f t="shared" si="0"/>
         <v>0.49460046205390207</v>
       </c>
       <c r="F6" s="1">
-        <f>D6/W6</f>
+        <f t="shared" si="1"/>
         <v>0.50539953794609793</v>
       </c>
       <c r="G6">
         <v>3330583</v>
       </c>
       <c r="H6">
-        <f>G6/W6</f>
+        <f t="shared" si="2"/>
         <v>0.2099466400234494</v>
       </c>
       <c r="I6">
         <v>3803904</v>
       </c>
       <c r="J6">
-        <f>I6/W6</f>
+        <f t="shared" si="3"/>
         <v>0.2397829040056228</v>
       </c>
       <c r="K6">
         <v>3063307</v>
       </c>
       <c r="L6">
-        <f>K6/W6</f>
+        <f t="shared" si="4"/>
         <v>0.19309862928211449</v>
       </c>
       <c r="M6">
         <v>2708223</v>
       </c>
       <c r="N6">
-        <f>M6/W6</f>
+        <f t="shared" si="5"/>
         <v>0.17071555318820344</v>
       </c>
       <c r="O6">
@@ -853,39 +853,39 @@
         <v>8212118</v>
       </c>
       <c r="E7">
-        <f>C7/W7</f>
+        <f t="shared" si="0"/>
         <v>0.49488855723743191</v>
       </c>
       <c r="F7" s="1">
-        <f>D7/W7</f>
+        <f t="shared" si="1"/>
         <v>0.50511144276256803</v>
       </c>
       <c r="G7">
         <v>3171481</v>
       </c>
       <c r="H7">
-        <f>G7/W7</f>
+        <f t="shared" si="2"/>
         <v>0.19507164212741124</v>
       </c>
       <c r="I7">
         <v>3887631</v>
       </c>
       <c r="J7">
-        <f>I7/W7</f>
+        <f t="shared" si="3"/>
         <v>0.23912063895556362</v>
       </c>
       <c r="K7">
         <v>3312214</v>
       </c>
       <c r="L7">
-        <f>K7/W7</f>
+        <f t="shared" si="4"/>
         <v>0.20372785586841016</v>
       </c>
       <c r="M7">
         <v>2857303</v>
       </c>
       <c r="N7">
-        <f>M7/W7</f>
+        <f t="shared" si="5"/>
         <v>0.17574716300226251</v>
       </c>
       <c r="O7">
@@ -898,15 +898,15 @@
         <v>6597240</v>
       </c>
       <c r="R7">
-        <f t="shared" ref="R7:R19" si="0">Q7/W7</f>
+        <f t="shared" ref="R7:R19" si="6">Q7/W7</f>
         <v>0.4057834306144803</v>
       </c>
       <c r="S7">
-        <f t="shared" ref="S7:S19" si="1">P7/W7</f>
+        <f t="shared" ref="S7:S19" si="7">P7/W7</f>
         <v>0.17826204303202256</v>
       </c>
       <c r="T7">
-        <f t="shared" ref="T7:T19" si="2">O7/W7</f>
+        <f t="shared" ref="T7:T19" si="8">O7/W7</f>
         <v>0.4159544033373781</v>
       </c>
       <c r="U7">
@@ -933,39 +933,39 @@
         <v>8269478</v>
       </c>
       <c r="E8">
-        <f>C8/W8</f>
+        <f t="shared" si="0"/>
         <v>0.49446863649279205</v>
       </c>
       <c r="F8" s="1">
-        <f>D8/W8</f>
+        <f t="shared" si="1"/>
         <v>0.50553136350720795</v>
       </c>
       <c r="G8">
         <v>3152682</v>
       </c>
       <c r="H8">
-        <f>G8/W8</f>
+        <f t="shared" si="2"/>
         <v>0.19273037913210864</v>
       </c>
       <c r="I8">
         <v>3731732</v>
       </c>
       <c r="J8">
-        <f>I8/W8</f>
+        <f t="shared" si="3"/>
         <v>0.22812897817776168</v>
       </c>
       <c r="K8">
         <v>3465142</v>
       </c>
       <c r="L8">
-        <f>K8/W8</f>
+        <f t="shared" si="4"/>
         <v>0.21183174560789614</v>
       </c>
       <c r="M8">
         <v>3034603</v>
       </c>
       <c r="N8">
-        <f>M8/W8</f>
+        <f t="shared" si="5"/>
         <v>0.18551195036652421</v>
       </c>
       <c r="O8">
@@ -978,15 +978,15 @@
         <v>6479490</v>
       </c>
       <c r="R8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.39610546331114477</v>
       </c>
       <c r="S8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0.18244170800425871</v>
       </c>
       <c r="T8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.42145331774217765</v>
       </c>
       <c r="U8">
@@ -1013,39 +1013,39 @@
         <v>8293326</v>
       </c>
       <c r="E9">
-        <f>C9/W9</f>
+        <f t="shared" si="0"/>
         <v>0.49447581250538314</v>
       </c>
       <c r="F9" s="1">
-        <f>D9/W9</f>
+        <f t="shared" si="1"/>
         <v>0.50552418749461692</v>
       </c>
       <c r="G9">
         <v>3168085</v>
       </c>
       <c r="H9">
-        <f>G9/W9</f>
+        <f t="shared" si="2"/>
         <v>0.19311234063859098</v>
       </c>
       <c r="I9">
         <v>3664878</v>
       </c>
       <c r="J9">
-        <f>I9/W9</f>
+        <f t="shared" si="3"/>
         <v>0.22339462758571127</v>
       </c>
       <c r="K9">
         <v>3461174</v>
       </c>
       <c r="L9">
-        <f>K9/W9</f>
+        <f t="shared" si="4"/>
         <v>0.21097773970630035</v>
       </c>
       <c r="M9">
         <v>3159434</v>
       </c>
       <c r="N9">
-        <f>M9/W9</f>
+        <f t="shared" si="5"/>
         <v>0.19258501423830046</v>
       </c>
       <c r="O9">
@@ -1058,15 +1058,15 @@
         <v>6435090</v>
       </c>
       <c r="R9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.39225440356555791</v>
       </c>
       <c r="S9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0.18295135644064495</v>
       </c>
       <c r="T9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.4247943009493399</v>
       </c>
       <c r="U9">
@@ -1093,39 +1093,39 @@
         <v>8329391</v>
       </c>
       <c r="E10">
-        <f>C10/W10</f>
+        <f t="shared" si="0"/>
         <v>0.49475320771765402</v>
       </c>
       <c r="F10" s="1">
-        <f>D10/W10</f>
+        <f t="shared" si="1"/>
         <v>0.50524679228234604</v>
       </c>
       <c r="G10">
         <v>3198736</v>
       </c>
       <c r="H10">
-        <f>G10/W10</f>
+        <f t="shared" si="2"/>
         <v>0.19402992407945099</v>
       </c>
       <c r="I10">
         <v>3603410</v>
       </c>
       <c r="J10">
-        <f>I10/W10</f>
+        <f t="shared" si="3"/>
         <v>0.21857676554962163</v>
       </c>
       <c r="K10">
         <v>3469734</v>
       </c>
       <c r="L10">
-        <f>K10/W10</f>
+        <f t="shared" si="4"/>
         <v>0.21046820512724082</v>
       </c>
       <c r="M10">
         <v>3274007</v>
       </c>
       <c r="N10">
-        <f>M10/W10</f>
+        <f t="shared" si="5"/>
         <v>0.19859573582990003</v>
       </c>
       <c r="O10">
@@ -1138,15 +1138,15 @@
         <v>6400880</v>
       </c>
       <c r="R10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.38826657168383893</v>
       </c>
       <c r="S10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0.18281080545320644</v>
       </c>
       <c r="T10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.42892219825477546</v>
       </c>
       <c r="U10">
@@ -1173,39 +1173,39 @@
         <v>8371513</v>
       </c>
       <c r="E11">
-        <f>C11/W11</f>
+        <f t="shared" si="0"/>
         <v>0.49493100719403194</v>
       </c>
       <c r="F11" s="1">
-        <f>D11/W11</f>
+        <f t="shared" si="1"/>
         <v>0.50506899280596806</v>
       </c>
       <c r="G11">
         <v>3226930</v>
       </c>
       <c r="H11">
-        <f>G11/W11</f>
+        <f t="shared" si="2"/>
         <v>0.19468670537277583</v>
       </c>
       <c r="I11">
         <v>3543886</v>
       </c>
       <c r="J11">
-        <f>I11/W11</f>
+        <f t="shared" si="3"/>
         <v>0.21380925200010692</v>
       </c>
       <c r="K11">
         <v>3497054</v>
       </c>
       <c r="L11">
-        <f>K11/W11</f>
+        <f t="shared" si="4"/>
         <v>0.21098379009482299</v>
       </c>
       <c r="M11">
         <v>3376242</v>
       </c>
       <c r="N11">
-        <f>M11/W11</f>
+        <f t="shared" si="5"/>
         <v>0.20369497681114601</v>
       </c>
       <c r="O11">
@@ -1218,15 +1218,15 @@
         <v>6353240</v>
       </c>
       <c r="R11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.38330281848150849</v>
       </c>
       <c r="S11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0.18190057320701691</v>
       </c>
       <c r="T11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.43479666864333966</v>
       </c>
       <c r="U11">
@@ -1253,39 +1253,39 @@
         <v>8412317</v>
       </c>
       <c r="E12">
-        <f>C12/W12</f>
+        <f t="shared" si="0"/>
         <v>0.4949316451285225</v>
       </c>
       <c r="F12" s="1">
-        <f>D12/W12</f>
+        <f t="shared" si="1"/>
         <v>0.5050683548714775</v>
       </c>
       <c r="G12">
         <v>3249228</v>
       </c>
       <c r="H12">
-        <f>G12/W12</f>
+        <f t="shared" si="2"/>
         <v>0.19508088444150892</v>
       </c>
       <c r="I12">
         <v>3476687</v>
       </c>
       <c r="J12">
-        <f>I12/W12</f>
+        <f t="shared" si="3"/>
         <v>0.20873732926291919</v>
       </c>
       <c r="K12">
         <v>3534552</v>
       </c>
       <c r="L12">
-        <f>K12/W12</f>
+        <f t="shared" si="4"/>
         <v>0.21221149462718661</v>
       </c>
       <c r="M12">
         <v>3469785</v>
       </c>
       <c r="N12">
-        <f>M12/W12</f>
+        <f t="shared" si="5"/>
         <v>0.20832293905564062</v>
       </c>
       <c r="O12">
@@ -1298,15 +1298,15 @@
         <v>6322030</v>
       </c>
       <c r="R12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.37956930195903543</v>
       </c>
       <c r="S12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0.18193363164384968</v>
       </c>
       <c r="T12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.43849712643626404</v>
       </c>
       <c r="U12">
@@ -1333,39 +1333,39 @@
         <v>8472236</v>
       </c>
       <c r="E13">
-        <f>C13/W13</f>
+        <f t="shared" si="0"/>
         <v>0.49508637733673233</v>
       </c>
       <c r="F13" s="1">
-        <f>D13/W13</f>
+        <f t="shared" si="1"/>
         <v>0.50491362266326767</v>
       </c>
       <c r="G13">
         <v>3271797</v>
       </c>
       <c r="H13">
-        <f>G13/W13</f>
+        <f t="shared" si="2"/>
         <v>0.1949868813721444</v>
       </c>
       <c r="I13">
         <v>3365064</v>
       </c>
       <c r="J13">
-        <f>I13/W13</f>
+        <f t="shared" si="3"/>
         <v>0.2005452462294188</v>
       </c>
       <c r="K13">
         <v>3603459</v>
       </c>
       <c r="L13">
-        <f>K13/W13</f>
+        <f t="shared" si="4"/>
         <v>0.21475269784842585</v>
       </c>
       <c r="M13">
         <v>3641612</v>
       </c>
       <c r="N13">
-        <f>M13/W13</f>
+        <f t="shared" si="5"/>
         <v>0.21702647415086496</v>
       </c>
       <c r="O13">
@@ -1378,15 +1378,15 @@
         <v>6237780</v>
       </c>
       <c r="R13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.37174839052836561</v>
       </c>
       <c r="S13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0.17918451450647588</v>
       </c>
       <c r="T13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.44906679698383301</v>
       </c>
       <c r="U13">
@@ -1413,39 +1413,39 @@
         <v>8494904</v>
       </c>
       <c r="E14">
-        <f>C14/W14</f>
+        <f t="shared" si="0"/>
         <v>0.49523096311436565</v>
       </c>
       <c r="F14" s="1">
-        <f>D14/W14</f>
+        <f t="shared" si="1"/>
         <v>0.50476903688563435</v>
       </c>
       <c r="G14">
         <v>3292799</v>
       </c>
       <c r="H14">
-        <f>G14/W14</f>
+        <f t="shared" si="2"/>
         <v>0.19565883026906247</v>
       </c>
       <c r="I14">
         <v>3308554</v>
       </c>
       <c r="J14">
-        <f>I14/W14</f>
+        <f t="shared" si="3"/>
         <v>0.19659499578383852</v>
       </c>
       <c r="K14">
         <v>3628031</v>
       </c>
       <c r="L14">
-        <f>K14/W14</f>
+        <f t="shared" si="4"/>
         <v>0.21557838836804097</v>
       </c>
       <c r="M14">
         <v>3729913</v>
       </c>
       <c r="N14">
-        <f>M14/W14</f>
+        <f t="shared" si="5"/>
         <v>0.22163223889018721</v>
       </c>
       <c r="O14">
@@ -1458,15 +1458,15 @@
         <v>6214070</v>
       </c>
       <c r="R14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.36924138625226532</v>
       </c>
       <c r="S14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0.1791905766191311</v>
       </c>
       <c r="T14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.45156809654882035</v>
       </c>
       <c r="U14">
@@ -1493,39 +1493,39 @@
         <v>8606405</v>
       </c>
       <c r="E15">
-        <f>C15/W15</f>
+        <f t="shared" si="0"/>
         <v>0.49615657447554246</v>
       </c>
       <c r="F15" s="1">
-        <f>D15/W15</f>
+        <f t="shared" si="1"/>
         <v>0.50384342552445749</v>
       </c>
       <c r="G15">
         <v>3405654</v>
       </c>
       <c r="H15">
-        <f>G15/W15</f>
+        <f t="shared" si="2"/>
         <v>0.19937667092253628</v>
       </c>
       <c r="I15">
         <v>3159640</v>
       </c>
       <c r="J15">
-        <f>I15/W15</f>
+        <f t="shared" si="3"/>
         <v>0.18497431169275638</v>
       </c>
       <c r="K15">
         <v>3729288</v>
       </c>
       <c r="L15">
-        <f>K15/W15</f>
+        <f t="shared" si="4"/>
         <v>0.21832312570547785</v>
       </c>
       <c r="M15">
         <v>4002932</v>
       </c>
       <c r="N15">
-        <f>M15/W15</f>
+        <f t="shared" si="5"/>
         <v>0.23434302371564758</v>
       </c>
       <c r="O15">
@@ -1538,15 +1538,15 @@
         <v>5916720</v>
       </c>
       <c r="R15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.34638161609511386</v>
       </c>
       <c r="S15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0.17336585115118941</v>
       </c>
       <c r="T15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.48025270838222878</v>
       </c>
       <c r="U15">
@@ -1573,39 +1573,39 @@
         <v>8701077</v>
       </c>
       <c r="E16">
-        <f>C16/W16</f>
+        <f t="shared" si="0"/>
         <v>0.4965284727380479</v>
       </c>
       <c r="F16" s="1">
-        <f>D16/W16</f>
+        <f t="shared" si="1"/>
         <v>0.5034715272619521</v>
       </c>
       <c r="G16">
         <v>3472436</v>
       </c>
       <c r="H16">
-        <f>G16/W16</f>
+        <f t="shared" si="2"/>
         <v>0.20092600677357342</v>
       </c>
       <c r="I16">
         <v>3135601</v>
       </c>
       <c r="J16">
-        <f>I16/W16</f>
+        <f t="shared" si="3"/>
         <v>0.18143568024442311</v>
       </c>
       <c r="K16">
         <v>3753725</v>
       </c>
       <c r="L16">
-        <f>K16/W16</f>
+        <f t="shared" si="4"/>
         <v>0.21720226802628814</v>
       </c>
       <c r="M16">
         <v>4178393</v>
       </c>
       <c r="N16">
-        <f>M16/W16</f>
+        <f t="shared" si="5"/>
         <v>0.24177488662732785</v>
       </c>
       <c r="O16">
@@ -1618,15 +1618,15 @@
         <v>5908730</v>
       </c>
       <c r="R16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.3418975969616766</v>
       </c>
       <c r="S16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0.17099942871734283</v>
       </c>
       <c r="T16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.48710280073159823</v>
       </c>
       <c r="U16">
@@ -1653,39 +1653,39 @@
         <v>8759554</v>
       </c>
       <c r="E17">
-        <f>C17/W17</f>
+        <f t="shared" si="0"/>
         <v>0.49679671246758239</v>
       </c>
       <c r="F17" s="1">
-        <f>D17/W17</f>
+        <f t="shared" si="1"/>
         <v>0.50320328753241761</v>
       </c>
       <c r="G17">
         <v>3506775</v>
       </c>
       <c r="H17">
-        <f>G17/W17</f>
+        <f t="shared" si="2"/>
         <v>0.20145097668631232</v>
       </c>
       <c r="I17">
         <v>3160047</v>
       </c>
       <c r="J17">
-        <f>I17/W17</f>
+        <f t="shared" si="3"/>
         <v>0.18153276287319578</v>
       </c>
       <c r="K17">
         <v>3740474</v>
       </c>
       <c r="L17">
-        <f>K17/W17</f>
+        <f t="shared" si="4"/>
         <v>0.21487610142360355</v>
       </c>
       <c r="M17">
         <v>4271792</v>
       </c>
       <c r="N17">
-        <f>M17/W17</f>
+        <f t="shared" si="5"/>
         <v>0.24539831343635549</v>
       </c>
       <c r="O17">
@@ -1698,15 +1698,15 @@
         <v>5900770</v>
       </c>
       <c r="R17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.33897694596924272</v>
       </c>
       <c r="S17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0.17067847148240264</v>
       </c>
       <c r="T17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.49034486977946684</v>
       </c>
       <c r="U17">
@@ -1733,39 +1733,39 @@
         <v>8788879</v>
       </c>
       <c r="E18">
-        <f>C18/W18</f>
+        <f t="shared" si="0"/>
         <v>0.49707180058384881</v>
       </c>
       <c r="F18" s="1">
-        <f>D18/W18</f>
+        <f t="shared" si="1"/>
         <v>0.50292819941615119</v>
       </c>
       <c r="G18">
         <v>3505536</v>
       </c>
       <c r="H18">
-        <f>G18/W18</f>
+        <f t="shared" si="2"/>
         <v>0.20059815460748714</v>
       </c>
       <c r="I18">
         <v>3186391</v>
       </c>
       <c r="J18">
-        <f>I18/W18</f>
+        <f t="shared" si="3"/>
         <v>0.18233564124228238</v>
       </c>
       <c r="K18">
         <v>3714479</v>
       </c>
       <c r="L18">
-        <f>K18/W18</f>
+        <f t="shared" si="4"/>
         <v>0.21255455163725726</v>
       </c>
       <c r="M18">
         <v>4354742</v>
       </c>
       <c r="N18">
-        <f>M18/W18</f>
+        <f t="shared" si="5"/>
         <v>0.24919247983524281</v>
       </c>
       <c r="O18">
@@ -1778,15 +1778,15 @@
         <v>5904110</v>
       </c>
       <c r="R18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.33785234857083507</v>
       </c>
       <c r="S18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0.16940656344928004</v>
       </c>
       <c r="T18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.49274137409612306</v>
       </c>
       <c r="U18">
@@ -1813,39 +1813,39 @@
         <v>8845204</v>
       </c>
       <c r="E19">
-        <f>C19/W19</f>
+        <f t="shared" si="0"/>
         <v>0.49716508840594609</v>
       </c>
       <c r="F19" s="1">
-        <f>D19/W19</f>
+        <f t="shared" si="1"/>
         <v>0.50283491159405391</v>
       </c>
       <c r="G19">
         <v>3527921</v>
       </c>
       <c r="H19">
-        <f>G19/W19</f>
+        <f t="shared" si="2"/>
         <v>0.20055635168457464</v>
       </c>
       <c r="I19">
         <v>3234546</v>
       </c>
       <c r="J19">
-        <f>I19/W19</f>
+        <f t="shared" si="3"/>
         <v>0.18387847832078275</v>
       </c>
       <c r="K19">
         <v>3675784</v>
       </c>
       <c r="L19">
-        <f>K19/W19</f>
+        <f t="shared" si="4"/>
         <v>0.20896211355654862</v>
       </c>
       <c r="M19">
         <v>4437365</v>
       </c>
       <c r="N19">
-        <f>M19/W19</f>
+        <f t="shared" si="5"/>
         <v>0.2522567074185682</v>
       </c>
       <c r="O19">
@@ -1858,15 +1858,15 @@
         <v>5908320</v>
       </c>
       <c r="R19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.3358780153481345</v>
       </c>
       <c r="S19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0.16922207406288969</v>
       </c>
       <c r="T19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.49490036537546717</v>
       </c>
       <c r="U19">

</xml_diff>

<commit_message>
Working on tables and plots
</commit_message>
<xml_diff>
--- a/data/all_waves/weigh_data.xlsx
+++ b/data/all_waves/weigh_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anuschka/Documents/climatechange/climatechange/data/all_waves/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9127283F-11D7-1440-9FC1-7025A53D1BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E31B10C-BACD-FA42-BCE2-0FE8C78662B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="15700" xr2:uid="{589232E4-3D71-D747-A62A-14D4E3B0C8AE}"/>
   </bookViews>
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9464F51-D6CA-254C-B404-8BB877CB06E8}">
   <dimension ref="A1:W19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="U26" sqref="U26"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>